<commit_message>
:poop: Save encore mais là avec date OK
</commit_message>
<xml_diff>
--- a/assets/InputData.xlsx
+++ b/assets/InputData.xlsx
@@ -11,6 +11,40 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>bertrand</author>
+  </authors>
+  <commentList>
+    <comment ref="A40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>bertrand:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Passage au compteur Linky</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -144,7 +178,7 @@
     <numFmt numFmtId="167" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -201,6 +235,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -242,7 +289,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -346,6 +393,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1085,8 +1135,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tabSuiviConso" displayName="tabSuiviConso" ref="A3:AE37" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
-  <autoFilter ref="A3:AE37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tabSuiviConso" displayName="tabSuiviConso" ref="A3:AE41" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="A3:AE41"/>
   <tableColumns count="31">
     <tableColumn id="1" name="Date" dataDxfId="30"/>
     <tableColumn id="24" name="Année" dataDxfId="29">
@@ -1484,17 +1534,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:AE37"/>
+  <dimension ref="A1:AE41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="23" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="T1" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A38" sqref="A38:XFD96"/>
+      <selection pane="bottomRight" activeCell="R50" sqref="R50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1557,30 +1607,30 @@
       <c r="U1" s="31"/>
       <c r="V1" s="31"/>
       <c r="W1" s="4"/>
-      <c r="AA1" s="5">
+      <c r="AA1" s="5" t="e">
         <f>PERCENTILE(tabSuiviConso[Conso HP + HC / jour_x000D_
 Instantané],0.9)</f>
-        <v>76.861244019637553</v>
-      </c>
-      <c r="AB1" s="5">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB1" s="5" t="e">
         <f>QUARTILE(tabSuiviConso[Conso HP + HC / jour_x000D_
 Instantané],1)</f>
-        <v>51.798561151426199</v>
-      </c>
-      <c r="AC1" s="5">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC1" s="5" t="e">
         <f>QUARTILE(tabSuiviConso[Conso HP + HC / jour_x000D_
 Instantané],2)</f>
-        <v>56.748768473036577</v>
-      </c>
-      <c r="AD1" s="5">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD1" s="5" t="e">
         <f>QUARTILE(tabSuiviConso[Conso HP + HC / jour_x000D_
 Instantané],3)</f>
-        <v>67.509846827142084</v>
-      </c>
-      <c r="AE1" s="5">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE1" s="5" t="e">
         <f>QUARTILE(tabSuiviConso[Conso HP + HC / jour_x000D_
 Instantané],4)</f>
-        <v>81.777777777777771</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:31" s="23" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
@@ -6452,9 +6502,9 @@
 Instantané]])</f>
         <v>52.774869109690314</v>
       </c>
-      <c r="S37" s="10">
-        <f>SUM($Q$4:Q37)</f>
-        <v>2230</v>
+      <c r="S37" s="32">
+        <f>SUM($Q$4:Q41)</f>
+        <v>-179759</v>
       </c>
       <c r="T37" s="21">
         <v>120482</v>
@@ -6471,9 +6521,9 @@
 Instantané]])</f>
         <v>0</v>
       </c>
-      <c r="W37" s="10">
-        <f>SUM($U$4:U37)</f>
-        <v>1050</v>
+      <c r="W37" s="32">
+        <f>SUM($U$4:U41)</f>
+        <v>-119432</v>
       </c>
       <c r="X37" s="5">
         <f>tabSuiviConso[[#This Row],[Diff HP
@@ -6485,7 +6535,7 @@
         <f>tabSuiviConso[[#This Row],[Diff HP
 cumul]]+tabSuiviConso[[#This Row],[Diff HC
 cumul]]</f>
-        <v>3280</v>
+        <v>-299191</v>
       </c>
       <c r="Z37" s="11">
         <f>tabSuiviConso[[#This Row],[HP + HC
@@ -6508,18 +6558,550 @@
         <f>tabSuiviConso[[#This Row],[HP + HC
 cumul]]/(tabSuiviConso[[#This Row],[Diff jour_x000D_
 Cumul]]*24)</f>
-        <v>2.7302239116563634</v>
+        <v>-249.04220193670091</v>
       </c>
       <c r="AD37" s="11">
         <f>tabSuiviConso[[#This Row],[HP + HC
 cumul]]/tabSuiviConso[[#This Row],[Diff jour_x000D_
 Cumul]]</f>
-        <v>65.525373879752721</v>
+        <v>-5977.0128464808222</v>
       </c>
       <c r="AE37" s="11">
         <f>tabSuiviConso[[#This Row],[Conso HP + HC / jour_x000D_
 cumul]]*365</f>
-        <v>23916.761466109743</v>
+        <v>-2181609.6889655003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>44909.321527777778</v>
+      </c>
+      <c r="B38" s="12">
+        <f>YEAR(tabSuiviConso[[#This Row],[Date]])</f>
+        <v>2022</v>
+      </c>
+      <c r="C38" s="12" t="str">
+        <f>IF(B39&lt;&gt;tabSuiviConso[[#This Row],[Année]],tabSuiviConso[[#This Row],[Année]],"")</f>
+        <v/>
+      </c>
+      <c r="D38" s="12">
+        <f>MONTH(tabSuiviConso[[#This Row],[Date]])</f>
+        <v>12</v>
+      </c>
+      <c r="E38" s="12">
+        <f>DAY(tabSuiviConso[[#This Row],[Date]])</f>
+        <v>14</v>
+      </c>
+      <c r="F38" s="12" t="str">
+        <f>TEXT(tabSuiviConso[[#This Row],[Date]]-1,"jjjj")</f>
+        <v>mardi</v>
+      </c>
+      <c r="G38" s="12" t="str">
+        <f>tabSuiviConso[[#This Row],[Mois]]&amp;"/"&amp;tabSuiviConso[[#This Row],[Année]]</f>
+        <v>12/2022</v>
+      </c>
+      <c r="H38" s="14" t="str">
+        <f>tabSuiviConso[[#This Row],[Jour]]&amp;"/"&amp;tabSuiviConso[[#This Row],[Mois]]&amp;"/"&amp;tabSuiviConso[[#This Row],[Année]]</f>
+        <v>14/12/2022</v>
+      </c>
+      <c r="I38" s="8">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A37),"",tabSuiviConso[[#This Row],[Date]]-A37)</f>
+        <v>676.55625000000146</v>
+      </c>
+      <c r="J38" s="9">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A37),"",tabSuiviConso[[#This Row],[Date]]-A37)</f>
+        <v>676.55625000000146</v>
+      </c>
+      <c r="K38" s="8">
+        <f>tabSuiviConso[[#This Row],[Date]]-$A$4</f>
+        <v>726.61319444444234</v>
+      </c>
+      <c r="L38" s="9">
+        <f>tabSuiviConso[[#This Row],[Date]]-$A$4</f>
+        <v>726.61319444444234</v>
+      </c>
+      <c r="O38" s="5">
+        <f>tabSuiviConso[[#This Row],[Max]]-tabSuiviConso[[#This Row],[Min]]</f>
+        <v>0</v>
+      </c>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Index HP
+kWh]]-P37),"",tabSuiviConso[[#This Row],[Index HP
+kWh]]-P37)</f>
+        <v>-181989</v>
+      </c>
+      <c r="R38" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A38),"",tabSuiviConso[[#This Row],[Diff HP
+instantannée]]/tabSuiviConso[[#This Row],[Diff jour
+Instantané]])</f>
+        <v>-268.99315467117424</v>
+      </c>
+      <c r="S38" s="5">
+        <f>SUM($Q$4:Q38)</f>
+        <v>-179759</v>
+      </c>
+      <c r="T38" s="21"/>
+      <c r="U38" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Index HC_x000D_
+kWh]]-T37),"",tabSuiviConso[[#This Row],[Index HC_x000D_
+kWh]]-T37)</f>
+        <v>-120482</v>
+      </c>
+      <c r="V38" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A38),"",tabSuiviConso[[#This Row],[Diff HC
+instantannée]]/tabSuiviConso[[#This Row],[Diff jour
+Instantané]])</f>
+        <v>-178.08127557760309</v>
+      </c>
+      <c r="W38" s="5">
+        <f>SUM($U$4:U38)</f>
+        <v>-119432</v>
+      </c>
+      <c r="X38" s="5">
+        <f>tabSuiviConso[[#This Row],[Diff HP
+instantannée]]+tabSuiviConso[[#This Row],[Diff HC
+instantannée]]</f>
+        <v>-302471</v>
+      </c>
+      <c r="Y38" s="5">
+        <f>tabSuiviConso[[#This Row],[Diff HP
+cumul]]+tabSuiviConso[[#This Row],[Diff HC
+cumul]]</f>
+        <v>-299191</v>
+      </c>
+      <c r="Z38" s="5">
+        <f>tabSuiviConso[[#This Row],[HP + HC
+instantanné]]/(tabSuiviConso[[#This Row],[Diff jour
+Instantané]]*24)</f>
+        <v>-18.628101260365721</v>
+      </c>
+      <c r="AA38" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A38),"",tabSuiviConso[[#This Row],[HP + HC
+instantanné]]/tabSuiviConso[[#This Row],[Diff jour
+Instantané]])</f>
+        <v>-447.07443024877733</v>
+      </c>
+      <c r="AB38" s="5">
+        <f>tabSuiviConso[[#This Row],[Conso HP + HC / jour_x000D_
+Instantané]]*365</f>
+        <v>-163182.16704080373</v>
+      </c>
+      <c r="AC38" s="5">
+        <f>tabSuiviConso[[#This Row],[HP + HC
+cumul]]/(tabSuiviConso[[#This Row],[Diff jour_x000D_
+Cumul]]*24)</f>
+        <v>-17.156709734948052</v>
+      </c>
+      <c r="AD38" s="5">
+        <f>tabSuiviConso[[#This Row],[HP + HC
+cumul]]/tabSuiviConso[[#This Row],[Diff jour_x000D_
+Cumul]]</f>
+        <v>-411.7610336387533</v>
+      </c>
+      <c r="AE38" s="5">
+        <f>tabSuiviConso[[#This Row],[Conso HP + HC / jour_x000D_
+cumul]]*365</f>
+        <v>-150292.77727814496</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>44910.34097222222</v>
+      </c>
+      <c r="B39" s="12">
+        <f>YEAR(tabSuiviConso[[#This Row],[Date]])</f>
+        <v>2022</v>
+      </c>
+      <c r="C39" s="12" t="str">
+        <f>IF(B40&lt;&gt;tabSuiviConso[[#This Row],[Année]],tabSuiviConso[[#This Row],[Année]],"")</f>
+        <v/>
+      </c>
+      <c r="D39" s="12">
+        <f>MONTH(tabSuiviConso[[#This Row],[Date]])</f>
+        <v>12</v>
+      </c>
+      <c r="E39" s="12">
+        <f>DAY(tabSuiviConso[[#This Row],[Date]])</f>
+        <v>15</v>
+      </c>
+      <c r="F39" s="12" t="str">
+        <f>TEXT(tabSuiviConso[[#This Row],[Date]]-1,"jjjj")</f>
+        <v>mercredi</v>
+      </c>
+      <c r="G39" s="12" t="str">
+        <f>tabSuiviConso[[#This Row],[Mois]]&amp;"/"&amp;tabSuiviConso[[#This Row],[Année]]</f>
+        <v>12/2022</v>
+      </c>
+      <c r="H39" s="14" t="str">
+        <f>tabSuiviConso[[#This Row],[Jour]]&amp;"/"&amp;tabSuiviConso[[#This Row],[Mois]]&amp;"/"&amp;tabSuiviConso[[#This Row],[Année]]</f>
+        <v>15/12/2022</v>
+      </c>
+      <c r="I39" s="8">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A38),"",tabSuiviConso[[#This Row],[Date]]-A38)</f>
+        <v>1.0194444444423425</v>
+      </c>
+      <c r="J39" s="9">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A38),"",tabSuiviConso[[#This Row],[Date]]-A38)</f>
+        <v>1.0194444444423425</v>
+      </c>
+      <c r="K39" s="8">
+        <f>tabSuiviConso[[#This Row],[Date]]-$A$4</f>
+        <v>727.63263888888469</v>
+      </c>
+      <c r="L39" s="9">
+        <f>tabSuiviConso[[#This Row],[Date]]-$A$4</f>
+        <v>727.63263888888469</v>
+      </c>
+      <c r="O39" s="5">
+        <f>tabSuiviConso[[#This Row],[Max]]-tabSuiviConso[[#This Row],[Min]]</f>
+        <v>0</v>
+      </c>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Index HP
+kWh]]-P38),"",tabSuiviConso[[#This Row],[Index HP
+kWh]]-P38)</f>
+        <v>0</v>
+      </c>
+      <c r="R39" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A39),"",tabSuiviConso[[#This Row],[Diff HP
+instantannée]]/tabSuiviConso[[#This Row],[Diff jour
+Instantané]])</f>
+        <v>0</v>
+      </c>
+      <c r="S39" s="5">
+        <f>SUM($Q$4:Q39)</f>
+        <v>-179759</v>
+      </c>
+      <c r="T39" s="21"/>
+      <c r="U39" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Index HC_x000D_
+kWh]]-T38),"",tabSuiviConso[[#This Row],[Index HC_x000D_
+kWh]]-T38)</f>
+        <v>0</v>
+      </c>
+      <c r="V39" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A39),"",tabSuiviConso[[#This Row],[Diff HC
+instantannée]]/tabSuiviConso[[#This Row],[Diff jour
+Instantané]])</f>
+        <v>0</v>
+      </c>
+      <c r="W39" s="5">
+        <f>SUM($U$4:U39)</f>
+        <v>-119432</v>
+      </c>
+      <c r="X39" s="5">
+        <f>tabSuiviConso[[#This Row],[Diff HP
+instantannée]]+tabSuiviConso[[#This Row],[Diff HC
+instantannée]]</f>
+        <v>0</v>
+      </c>
+      <c r="Y39" s="5">
+        <f>tabSuiviConso[[#This Row],[Diff HP
+cumul]]+tabSuiviConso[[#This Row],[Diff HC
+cumul]]</f>
+        <v>-299191</v>
+      </c>
+      <c r="Z39" s="5">
+        <f>tabSuiviConso[[#This Row],[HP + HC
+instantanné]]/(tabSuiviConso[[#This Row],[Diff jour
+Instantané]]*24)</f>
+        <v>0</v>
+      </c>
+      <c r="AA39" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A39),"",tabSuiviConso[[#This Row],[HP + HC
+instantanné]]/tabSuiviConso[[#This Row],[Diff jour
+Instantané]])</f>
+        <v>0</v>
+      </c>
+      <c r="AB39" s="5">
+        <f>tabSuiviConso[[#This Row],[Conso HP + HC / jour_x000D_
+Instantané]]*365</f>
+        <v>0</v>
+      </c>
+      <c r="AC39" s="5">
+        <f>tabSuiviConso[[#This Row],[HP + HC
+cumul]]/(tabSuiviConso[[#This Row],[Diff jour_x000D_
+Cumul]]*24)</f>
+        <v>-17.132672450899182</v>
+      </c>
+      <c r="AD39" s="5">
+        <f>tabSuiviConso[[#This Row],[HP + HC
+cumul]]/tabSuiviConso[[#This Row],[Diff jour_x000D_
+Cumul]]</f>
+        <v>-411.18413882158035</v>
+      </c>
+      <c r="AE39" s="5">
+        <f>tabSuiviConso[[#This Row],[Conso HP + HC / jour_x000D_
+cumul]]*365</f>
+        <v>-150082.21066987683</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>44910.34097222222</v>
+      </c>
+      <c r="B40" s="12">
+        <f>YEAR(tabSuiviConso[[#This Row],[Date]])</f>
+        <v>2022</v>
+      </c>
+      <c r="C40" s="12" t="str">
+        <f>IF(B41&lt;&gt;tabSuiviConso[[#This Row],[Année]],tabSuiviConso[[#This Row],[Année]],"")</f>
+        <v/>
+      </c>
+      <c r="D40" s="12">
+        <f>MONTH(tabSuiviConso[[#This Row],[Date]])</f>
+        <v>12</v>
+      </c>
+      <c r="E40" s="12">
+        <f>DAY(tabSuiviConso[[#This Row],[Date]])</f>
+        <v>15</v>
+      </c>
+      <c r="F40" s="12" t="str">
+        <f>TEXT(tabSuiviConso[[#This Row],[Date]]-1,"jjjj")</f>
+        <v>mercredi</v>
+      </c>
+      <c r="G40" s="12" t="str">
+        <f>tabSuiviConso[[#This Row],[Mois]]&amp;"/"&amp;tabSuiviConso[[#This Row],[Année]]</f>
+        <v>12/2022</v>
+      </c>
+      <c r="H40" s="14" t="str">
+        <f>tabSuiviConso[[#This Row],[Jour]]&amp;"/"&amp;tabSuiviConso[[#This Row],[Mois]]&amp;"/"&amp;tabSuiviConso[[#This Row],[Année]]</f>
+        <v>15/12/2022</v>
+      </c>
+      <c r="I40" s="8">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A39),"",tabSuiviConso[[#This Row],[Date]]-A39)</f>
+        <v>0</v>
+      </c>
+      <c r="J40" s="9">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A39),"",tabSuiviConso[[#This Row],[Date]]-A39)</f>
+        <v>0</v>
+      </c>
+      <c r="K40" s="8">
+        <f>tabSuiviConso[[#This Row],[Date]]-$A$4</f>
+        <v>727.63263888888469</v>
+      </c>
+      <c r="L40" s="9">
+        <f>tabSuiviConso[[#This Row],[Date]]-$A$4</f>
+        <v>727.63263888888469</v>
+      </c>
+      <c r="O40" s="5">
+        <f>tabSuiviConso[[#This Row],[Max]]-tabSuiviConso[[#This Row],[Min]]</f>
+        <v>0</v>
+      </c>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Index HP
+kWh]]-P39),"",tabSuiviConso[[#This Row],[Index HP
+kWh]]-P39)</f>
+        <v>0</v>
+      </c>
+      <c r="R40" s="5" t="e">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A40),"",tabSuiviConso[[#This Row],[Diff HP
+instantannée]]/tabSuiviConso[[#This Row],[Diff jour
+Instantané]])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S40" s="5">
+        <f>SUM($Q$4:Q40)</f>
+        <v>-179759</v>
+      </c>
+      <c r="T40" s="21"/>
+      <c r="U40" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Index HC_x000D_
+kWh]]-T39),"",tabSuiviConso[[#This Row],[Index HC_x000D_
+kWh]]-T39)</f>
+        <v>0</v>
+      </c>
+      <c r="V40" s="5" t="e">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A40),"",tabSuiviConso[[#This Row],[Diff HC
+instantannée]]/tabSuiviConso[[#This Row],[Diff jour
+Instantané]])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W40" s="5">
+        <f>SUM($U$4:U40)</f>
+        <v>-119432</v>
+      </c>
+      <c r="X40" s="5">
+        <f>tabSuiviConso[[#This Row],[Diff HP
+instantannée]]+tabSuiviConso[[#This Row],[Diff HC
+instantannée]]</f>
+        <v>0</v>
+      </c>
+      <c r="Y40" s="5">
+        <f>tabSuiviConso[[#This Row],[Diff HP
+cumul]]+tabSuiviConso[[#This Row],[Diff HC
+cumul]]</f>
+        <v>-299191</v>
+      </c>
+      <c r="Z40" s="5" t="e">
+        <f>tabSuiviConso[[#This Row],[HP + HC
+instantanné]]/(tabSuiviConso[[#This Row],[Diff jour
+Instantané]]*24)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA40" s="5" t="e">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A40),"",tabSuiviConso[[#This Row],[HP + HC
+instantanné]]/tabSuiviConso[[#This Row],[Diff jour
+Instantané]])</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB40" s="5" t="e">
+        <f>tabSuiviConso[[#This Row],[Conso HP + HC / jour_x000D_
+Instantané]]*365</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC40" s="5">
+        <f>tabSuiviConso[[#This Row],[HP + HC
+cumul]]/(tabSuiviConso[[#This Row],[Diff jour_x000D_
+Cumul]]*24)</f>
+        <v>-17.132672450899182</v>
+      </c>
+      <c r="AD40" s="5">
+        <f>tabSuiviConso[[#This Row],[HP + HC
+cumul]]/tabSuiviConso[[#This Row],[Diff jour_x000D_
+Cumul]]</f>
+        <v>-411.18413882158035</v>
+      </c>
+      <c r="AE40" s="5">
+        <f>tabSuiviConso[[#This Row],[Conso HP + HC / jour_x000D_
+cumul]]*365</f>
+        <v>-150082.21066987683</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>44911.337500000001</v>
+      </c>
+      <c r="B41" s="12">
+        <f>YEAR(tabSuiviConso[[#This Row],[Date]])</f>
+        <v>2022</v>
+      </c>
+      <c r="C41" s="12">
+        <f>IF(B42&lt;&gt;tabSuiviConso[[#This Row],[Année]],tabSuiviConso[[#This Row],[Année]],"")</f>
+        <v>2022</v>
+      </c>
+      <c r="D41" s="12">
+        <f>MONTH(tabSuiviConso[[#This Row],[Date]])</f>
+        <v>12</v>
+      </c>
+      <c r="E41" s="12">
+        <f>DAY(tabSuiviConso[[#This Row],[Date]])</f>
+        <v>16</v>
+      </c>
+      <c r="F41" s="12" t="str">
+        <f>TEXT(tabSuiviConso[[#This Row],[Date]]-1,"jjjj")</f>
+        <v>jeudi</v>
+      </c>
+      <c r="G41" s="12" t="str">
+        <f>tabSuiviConso[[#This Row],[Mois]]&amp;"/"&amp;tabSuiviConso[[#This Row],[Année]]</f>
+        <v>12/2022</v>
+      </c>
+      <c r="H41" s="14" t="str">
+        <f>tabSuiviConso[[#This Row],[Jour]]&amp;"/"&amp;tabSuiviConso[[#This Row],[Mois]]&amp;"/"&amp;tabSuiviConso[[#This Row],[Année]]</f>
+        <v>16/12/2022</v>
+      </c>
+      <c r="I41" s="8">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A40),"",tabSuiviConso[[#This Row],[Date]]-A40)</f>
+        <v>0.99652777778101154</v>
+      </c>
+      <c r="J41" s="9">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A40),"",tabSuiviConso[[#This Row],[Date]]-A40)</f>
+        <v>0.99652777778101154</v>
+      </c>
+      <c r="K41" s="8">
+        <f>tabSuiviConso[[#This Row],[Date]]-$A$4</f>
+        <v>728.6291666666657</v>
+      </c>
+      <c r="L41" s="9">
+        <f>tabSuiviConso[[#This Row],[Date]]-$A$4</f>
+        <v>728.6291666666657</v>
+      </c>
+      <c r="O41" s="5">
+        <f>tabSuiviConso[[#This Row],[Max]]-tabSuiviConso[[#This Row],[Min]]</f>
+        <v>0</v>
+      </c>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Index HP
+kWh]]-P40),"",tabSuiviConso[[#This Row],[Index HP
+kWh]]-P40)</f>
+        <v>0</v>
+      </c>
+      <c r="R41" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A41),"",tabSuiviConso[[#This Row],[Diff HP
+instantannée]]/tabSuiviConso[[#This Row],[Diff jour
+Instantané]])</f>
+        <v>0</v>
+      </c>
+      <c r="S41" s="5">
+        <f>SUM($Q$4:Q41)</f>
+        <v>-179759</v>
+      </c>
+      <c r="T41" s="21"/>
+      <c r="U41" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Index HC_x000D_
+kWh]]-T40),"",tabSuiviConso[[#This Row],[Index HC_x000D_
+kWh]]-T40)</f>
+        <v>0</v>
+      </c>
+      <c r="V41" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A41),"",tabSuiviConso[[#This Row],[Diff HC
+instantannée]]/tabSuiviConso[[#This Row],[Diff jour
+Instantané]])</f>
+        <v>0</v>
+      </c>
+      <c r="W41" s="5">
+        <f>SUM($U$4:U41)</f>
+        <v>-119432</v>
+      </c>
+      <c r="X41" s="5">
+        <f>tabSuiviConso[[#This Row],[Diff HP
+instantannée]]+tabSuiviConso[[#This Row],[Diff HC
+instantannée]]</f>
+        <v>0</v>
+      </c>
+      <c r="Y41" s="5">
+        <f>tabSuiviConso[[#This Row],[Diff HP
+cumul]]+tabSuiviConso[[#This Row],[Diff HC
+cumul]]</f>
+        <v>-299191</v>
+      </c>
+      <c r="Z41" s="5">
+        <f>tabSuiviConso[[#This Row],[HP + HC
+instantanné]]/(tabSuiviConso[[#This Row],[Diff jour
+Instantané]]*24)</f>
+        <v>0</v>
+      </c>
+      <c r="AA41" s="5">
+        <f>IF(ISERROR(tabSuiviConso[[#This Row],[Date]]-A41),"",tabSuiviConso[[#This Row],[HP + HC
+instantanné]]/tabSuiviConso[[#This Row],[Diff jour
+Instantané]])</f>
+        <v>0</v>
+      </c>
+      <c r="AB41" s="5">
+        <f>tabSuiviConso[[#This Row],[Conso HP + HC / jour_x000D_
+Instantané]]*365</f>
+        <v>0</v>
+      </c>
+      <c r="AC41" s="5">
+        <f>tabSuiviConso[[#This Row],[HP + HC
+cumul]]/(tabSuiviConso[[#This Row],[Diff jour_x000D_
+Cumul]]*24)</f>
+        <v>-17.109240525873382</v>
+      </c>
+      <c r="AD41" s="5">
+        <f>tabSuiviConso[[#This Row],[HP + HC
+cumul]]/tabSuiviConso[[#This Row],[Diff jour_x000D_
+Cumul]]</f>
+        <v>-410.62177262096117</v>
+      </c>
+      <c r="AE41" s="5">
+        <f>tabSuiviConso[[#This Row],[Conso HP + HC / jour_x000D_
+cumul]]*365</f>
+        <v>-149876.94700665082</v>
       </c>
     </row>
   </sheetData>
@@ -6529,8 +7111,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>